<commit_message>
SQL updated in sheet
</commit_message>
<xml_diff>
--- a/documents/SQL-queries in a sheet.xlsx
+++ b/documents/SQL-queries in a sheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="189">
   <si>
     <t>/* Class */</t>
   </si>
@@ -125,9 +125,6 @@
     <t>'t',</t>
   </si>
   <si>
-    <t>/*Test has Question*/</t>
-  </si>
-  <si>
     <t>test_has_question</t>
   </si>
   <si>
@@ -579,6 +576,21 @@
   </si>
   <si>
     <t>INSERT INTO user_answers_alternative VALUES ('bob@student.com',' 42');</t>
+  </si>
+  <si>
+    <t>/*Tests*/</t>
+  </si>
+  <si>
+    <t>Coding genius'</t>
+  </si>
+  <si>
+    <t>General coolness'</t>
+  </si>
+  <si>
+    <t>Random awsome'</t>
+  </si>
+  <si>
+    <t>Geek party trix'</t>
   </si>
 </sst>
 </file>
@@ -620,10 +632,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -904,10 +919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O206"/>
+  <dimension ref="A1:O211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A120" sqref="A120:A178"/>
+      <selection activeCell="A21" sqref="A21:J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1128,13 +1143,13 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
@@ -1142,46 +1157,31 @@
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>36</v>
-      </c>
-      <c r="F23" t="s">
-        <v>37</v>
+        <v>109</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="G23" t="s">
-        <v>38</v>
-      </c>
-      <c r="H23" t="s">
-        <v>39</v>
+        <v>111</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>185</v>
       </c>
       <c r="I23" t="s">
-        <v>11</v>
-      </c>
-      <c r="J23" t="s">
-        <v>110</v>
-      </c>
-      <c r="K23" t="s">
-        <v>111</v>
-      </c>
-      <c r="L23" t="s">
-        <v>112</v>
-      </c>
-      <c r="M23" t="s">
-        <v>111</v>
-      </c>
-      <c r="N23" t="s">
-        <v>39</v>
-      </c>
-      <c r="O23" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
@@ -1189,46 +1189,31 @@
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>36</v>
-      </c>
-      <c r="F24" t="s">
-        <v>37</v>
+        <v>109</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="G24" t="s">
-        <v>38</v>
-      </c>
-      <c r="H24" t="s">
-        <v>39</v>
+        <v>111</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>186</v>
       </c>
       <c r="I24" t="s">
-        <v>11</v>
-      </c>
-      <c r="J24" t="s">
-        <v>110</v>
-      </c>
-      <c r="K24" t="s">
-        <v>111</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="M24" t="s">
-        <v>116</v>
-      </c>
-      <c r="N24" t="s">
-        <v>39</v>
-      </c>
-      <c r="O24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>8</v>
       </c>
@@ -1236,46 +1221,31 @@
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>36</v>
-      </c>
-      <c r="F25" t="s">
-        <v>37</v>
+        <v>109</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="G25" t="s">
-        <v>38</v>
-      </c>
-      <c r="H25" t="s">
-        <v>39</v>
+        <v>111</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>187</v>
       </c>
       <c r="I25" t="s">
-        <v>11</v>
-      </c>
-      <c r="J25" t="s">
-        <v>110</v>
-      </c>
-      <c r="K25" t="s">
-        <v>111</v>
-      </c>
-      <c r="L25" t="s">
-        <v>112</v>
-      </c>
-      <c r="M25" t="s">
-        <v>113</v>
-      </c>
-      <c r="N25" t="s">
-        <v>39</v>
-      </c>
-      <c r="O25" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>8</v>
       </c>
@@ -1283,90 +1253,28 @@
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="E26" t="s">
-        <v>36</v>
-      </c>
-      <c r="F26" t="s">
-        <v>37</v>
+        <v>109</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="G26" t="s">
-        <v>38</v>
-      </c>
-      <c r="H26" t="s">
-        <v>39</v>
+        <v>111</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="I26" t="s">
-        <v>11</v>
-      </c>
-      <c r="J26" t="s">
-        <v>110</v>
-      </c>
-      <c r="K26" t="s">
-        <v>111</v>
-      </c>
-      <c r="L26" t="s">
-        <v>112</v>
-      </c>
-      <c r="M26" t="s">
-        <v>114</v>
-      </c>
-      <c r="N26" t="s">
-        <v>39</v>
-      </c>
-      <c r="O26" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" t="s">
-        <v>36</v>
-      </c>
-      <c r="F27" t="s">
-        <v>37</v>
-      </c>
-      <c r="G27" t="s">
-        <v>38</v>
-      </c>
-      <c r="H27" t="s">
-        <v>39</v>
-      </c>
-      <c r="I27" t="s">
-        <v>11</v>
-      </c>
-      <c r="J27" t="s">
-        <v>110</v>
-      </c>
-      <c r="K27" t="s">
-        <v>111</v>
-      </c>
-      <c r="L27" t="s">
-        <v>112</v>
-      </c>
-      <c r="M27" t="s">
-        <v>115</v>
-      </c>
-      <c r="N27" t="s">
-        <v>39</v>
-      </c>
-      <c r="O27" t="s">
-        <v>103</v>
+        <v>38</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.45">
@@ -1377,43 +1285,43 @@
         <v>9</v>
       </c>
       <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" t="s">
         <v>34</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>35</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>36</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>37</v>
       </c>
-      <c r="G28" t="s">
-        <v>38</v>
-      </c>
       <c r="H28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I28" t="s">
         <v>11</v>
       </c>
       <c r="J28" t="s">
+        <v>109</v>
+      </c>
+      <c r="K28" t="s">
         <v>110</v>
       </c>
-      <c r="K28" t="s">
-        <v>116</v>
-      </c>
       <c r="L28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M28" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="N28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.45">
@@ -1424,43 +1332,43 @@
         <v>9</v>
       </c>
       <c r="C29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" t="s">
         <v>34</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>35</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>36</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>37</v>
       </c>
-      <c r="G29" t="s">
-        <v>38</v>
-      </c>
       <c r="H29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I29" t="s">
         <v>11</v>
       </c>
       <c r="J29" t="s">
+        <v>109</v>
+      </c>
+      <c r="K29" t="s">
         <v>110</v>
       </c>
-      <c r="K29" t="s">
-        <v>116</v>
-      </c>
-      <c r="L29" t="s">
-        <v>112</v>
+      <c r="L29" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="M29" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="N29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.45">
@@ -1471,43 +1379,43 @@
         <v>9</v>
       </c>
       <c r="C30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" t="s">
         <v>34</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>35</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>36</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>37</v>
       </c>
-      <c r="G30" t="s">
-        <v>38</v>
-      </c>
       <c r="H30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I30" t="s">
         <v>11</v>
       </c>
       <c r="J30" t="s">
+        <v>109</v>
+      </c>
+      <c r="K30" t="s">
         <v>110</v>
       </c>
-      <c r="K30" t="s">
-        <v>116</v>
-      </c>
       <c r="L30" t="s">
+        <v>111</v>
+      </c>
+      <c r="M30" t="s">
         <v>112</v>
       </c>
-      <c r="M30" t="s">
-        <v>119</v>
-      </c>
       <c r="N30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.45">
@@ -1518,43 +1426,43 @@
         <v>9</v>
       </c>
       <c r="C31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" t="s">
         <v>34</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>35</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>36</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>37</v>
       </c>
-      <c r="G31" t="s">
-        <v>38</v>
-      </c>
       <c r="H31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I31" t="s">
         <v>11</v>
       </c>
       <c r="J31" t="s">
+        <v>109</v>
+      </c>
+      <c r="K31" t="s">
         <v>110</v>
       </c>
-      <c r="K31" t="s">
-        <v>116</v>
-      </c>
       <c r="L31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M31" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="N31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.45">
@@ -1565,43 +1473,43 @@
         <v>9</v>
       </c>
       <c r="C32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" t="s">
         <v>34</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>35</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>36</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>37</v>
       </c>
-      <c r="G32" t="s">
-        <v>38</v>
-      </c>
       <c r="H32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I32" t="s">
         <v>11</v>
       </c>
       <c r="J32" t="s">
+        <v>109</v>
+      </c>
+      <c r="K32" t="s">
         <v>110</v>
       </c>
-      <c r="K32" t="s">
-        <v>116</v>
-      </c>
       <c r="L32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M32" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="N32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.45">
@@ -1612,43 +1520,43 @@
         <v>9</v>
       </c>
       <c r="C33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" t="s">
         <v>34</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>35</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>36</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>37</v>
       </c>
-      <c r="G33" t="s">
-        <v>38</v>
-      </c>
       <c r="H33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I33" t="s">
         <v>11</v>
       </c>
       <c r="J33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K33" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M33" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="N33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.45">
@@ -1659,43 +1567,43 @@
         <v>9</v>
       </c>
       <c r="C34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" t="s">
         <v>34</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>35</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>36</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>37</v>
       </c>
-      <c r="G34" t="s">
-        <v>38</v>
-      </c>
       <c r="H34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I34" t="s">
         <v>11</v>
       </c>
       <c r="J34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K34" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M34" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="N34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.45">
@@ -1706,43 +1614,43 @@
         <v>9</v>
       </c>
       <c r="C35" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" t="s">
         <v>34</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>35</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>36</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>37</v>
       </c>
-      <c r="G35" t="s">
-        <v>38</v>
-      </c>
       <c r="H35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I35" t="s">
         <v>11</v>
       </c>
       <c r="J35" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K35" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M35" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="N35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.45">
@@ -1753,43 +1661,43 @@
         <v>9</v>
       </c>
       <c r="C36" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" t="s">
         <v>34</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>35</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>36</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>37</v>
       </c>
-      <c r="G36" t="s">
-        <v>38</v>
-      </c>
       <c r="H36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I36" t="s">
         <v>11</v>
       </c>
       <c r="J36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K36" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M36" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="N36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O36" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.45">
@@ -1800,869 +1708,1104 @@
         <v>9</v>
       </c>
       <c r="C37" t="s">
+        <v>33</v>
+      </c>
+      <c r="D37" t="s">
         <v>34</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>35</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>36</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>37</v>
       </c>
-      <c r="G37" t="s">
-        <v>38</v>
-      </c>
       <c r="H37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I37" t="s">
         <v>11</v>
       </c>
       <c r="J37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K37" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L37" t="s">
+        <v>111</v>
+      </c>
+      <c r="M37" t="s">
+        <v>120</v>
+      </c>
+      <c r="N37" t="s">
+        <v>38</v>
+      </c>
+      <c r="O37" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" t="s">
+        <v>33</v>
+      </c>
+      <c r="D38" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38" t="s">
+        <v>35</v>
+      </c>
+      <c r="F38" t="s">
+        <v>36</v>
+      </c>
+      <c r="G38" t="s">
+        <v>37</v>
+      </c>
+      <c r="H38" t="s">
+        <v>38</v>
+      </c>
+      <c r="I38" t="s">
+        <v>11</v>
+      </c>
+      <c r="J38" t="s">
+        <v>109</v>
+      </c>
+      <c r="K38" t="s">
         <v>112</v>
       </c>
-      <c r="M37" t="s">
-        <v>126</v>
-      </c>
-      <c r="N37" t="s">
-        <v>39</v>
-      </c>
-      <c r="O37" t="s">
-        <v>103</v>
+      <c r="L38" t="s">
+        <v>111</v>
+      </c>
+      <c r="M38" t="s">
+        <v>121</v>
+      </c>
+      <c r="N38" t="s">
+        <v>38</v>
+      </c>
+      <c r="O38" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" t="s">
+        <v>33</v>
+      </c>
+      <c r="D39" t="s">
+        <v>34</v>
+      </c>
+      <c r="E39" t="s">
+        <v>35</v>
+      </c>
+      <c r="F39" t="s">
+        <v>36</v>
+      </c>
+      <c r="G39" t="s">
+        <v>37</v>
+      </c>
+      <c r="H39" t="s">
+        <v>38</v>
+      </c>
+      <c r="I39" t="s">
+        <v>11</v>
+      </c>
+      <c r="J39" t="s">
+        <v>109</v>
+      </c>
+      <c r="K39" t="s">
+        <v>112</v>
+      </c>
+      <c r="L39" t="s">
+        <v>111</v>
+      </c>
+      <c r="M39" t="s">
+        <v>122</v>
+      </c>
+      <c r="N39" t="s">
+        <v>38</v>
+      </c>
+      <c r="O39" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
-        <v>40</v>
+        <v>8</v>
+      </c>
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" t="s">
+        <v>34</v>
+      </c>
+      <c r="E40" t="s">
+        <v>35</v>
+      </c>
+      <c r="F40" t="s">
+        <v>36</v>
+      </c>
+      <c r="G40" t="s">
+        <v>37</v>
+      </c>
+      <c r="H40" t="s">
+        <v>38</v>
+      </c>
+      <c r="I40" t="s">
+        <v>11</v>
+      </c>
+      <c r="J40" t="s">
+        <v>109</v>
+      </c>
+      <c r="K40" t="s">
+        <v>112</v>
+      </c>
+      <c r="L40" t="s">
+        <v>111</v>
+      </c>
+      <c r="M40" t="s">
+        <v>123</v>
+      </c>
+      <c r="N40" t="s">
+        <v>38</v>
+      </c>
+      <c r="O40" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A41" s="1"/>
+      <c r="A41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" t="s">
+        <v>34</v>
+      </c>
+      <c r="E41" t="s">
+        <v>35</v>
+      </c>
+      <c r="F41" t="s">
+        <v>36</v>
+      </c>
+      <c r="G41" t="s">
+        <v>37</v>
+      </c>
+      <c r="H41" t="s">
+        <v>38</v>
+      </c>
+      <c r="I41" t="s">
+        <v>11</v>
+      </c>
+      <c r="J41" t="s">
+        <v>109</v>
+      </c>
+      <c r="K41" t="s">
+        <v>112</v>
+      </c>
+      <c r="L41" t="s">
+        <v>111</v>
+      </c>
+      <c r="M41" t="s">
+        <v>124</v>
+      </c>
+      <c r="N41" t="s">
+        <v>38</v>
+      </c>
+      <c r="O41" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A43" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A44" s="1" t="s">
-        <v>43</v>
+        <v>8</v>
+      </c>
+      <c r="B42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" t="s">
+        <v>34</v>
+      </c>
+      <c r="E42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F42" t="s">
+        <v>36</v>
+      </c>
+      <c r="G42" t="s">
+        <v>37</v>
+      </c>
+      <c r="H42" t="s">
+        <v>38</v>
+      </c>
+      <c r="I42" t="s">
+        <v>11</v>
+      </c>
+      <c r="J42" t="s">
+        <v>109</v>
+      </c>
+      <c r="K42" t="s">
+        <v>112</v>
+      </c>
+      <c r="L42" t="s">
+        <v>111</v>
+      </c>
+      <c r="M42" t="s">
+        <v>125</v>
+      </c>
+      <c r="N42" t="s">
+        <v>38</v>
+      </c>
+      <c r="O42" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A46" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="A46" s="1"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A57" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A59" s="1"/>
+      <c r="A59" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A61" s="1"/>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A62" s="1" t="s">
-        <v>58</v>
+      <c r="A61" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A64" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="A64" s="1"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A65" s="1"/>
+      <c r="A65" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A66" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="A66" s="1"/>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A69" s="1"/>
+      <c r="A69" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A70" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="A70" s="1"/>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A72" s="1"/>
+      <c r="A72" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A74" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="A74" s="1"/>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A75" s="1"/>
+      <c r="A75" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A77" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="A77" s="1"/>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A79" s="1"/>
+      <c r="A79" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A80" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="A80" s="1"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A83" s="1"/>
+      <c r="A83" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A84" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="A84" s="1"/>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A86" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A87" s="1"/>
+      <c r="A87" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A88" s="1" t="s">
-        <v>74</v>
-      </c>
+      <c r="A88" s="1"/>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A89" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A90" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A91" s="1"/>
+      <c r="A91" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A92" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="A92" s="1"/>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A93" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A94" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A95" s="1"/>
+      <c r="A95" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A96" s="1" t="s">
-        <v>80</v>
-      </c>
+      <c r="A96" s="1"/>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A97" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A98" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A99" s="1"/>
+      <c r="A99" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A100" s="1" t="s">
-        <v>83</v>
-      </c>
+      <c r="A100" s="1"/>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A101" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A102" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A103" s="1"/>
+      <c r="A103" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A104" s="1" t="s">
-        <v>86</v>
-      </c>
+      <c r="A104" s="1"/>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A105" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A106" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A107" s="1"/>
+      <c r="A107" s="1" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A108" s="1" t="s">
-        <v>89</v>
-      </c>
+      <c r="A108" s="1"/>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A109" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A110" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A111" s="1"/>
+      <c r="A111" s="1" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A112" s="1" t="s">
-        <v>92</v>
-      </c>
+      <c r="A112" s="1"/>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A113" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A114" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A115" s="1"/>
+      <c r="A115" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A116" s="1" t="s">
-        <v>95</v>
-      </c>
+      <c r="A116" s="1"/>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A117" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A118" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A119" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A120" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="A120" s="1"/>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A121" s="1"/>
+      <c r="A121" s="1" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A122" s="1" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A123" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A124" s="1" t="s">
-        <v>129</v>
+        <v>96</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A125" s="1"/>
+      <c r="A125" s="1" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A126" s="1" t="s">
-        <v>130</v>
-      </c>
+      <c r="A126" s="1"/>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A127" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A128" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A129" s="1"/>
+      <c r="A129" s="1" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A130" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="A130" s="1"/>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A131" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A132" s="1"/>
+      <c r="A132" s="1" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A133" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A134" s="1" t="s">
-        <v>136</v>
-      </c>
+      <c r="A134" s="1"/>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A135" s="1"/>
+      <c r="A135" s="1" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A136" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A137" s="1" t="s">
-        <v>138</v>
-      </c>
+      <c r="A137" s="1"/>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A138" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A139" s="1"/>
+      <c r="A139" s="1" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A140" s="1" t="s">
-        <v>140</v>
-      </c>
+      <c r="A140" s="1"/>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A141" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A142" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A143" s="1"/>
+      <c r="A143" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A144" s="1" t="s">
-        <v>143</v>
-      </c>
+      <c r="A144" s="1"/>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A145" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A146" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A147" s="1"/>
+      <c r="A147" s="1" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A148" s="1" t="s">
-        <v>146</v>
-      </c>
+      <c r="A148" s="1"/>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A149" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A150" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A151" s="1"/>
+      <c r="A151" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A152" s="1" t="s">
-        <v>149</v>
-      </c>
+      <c r="A152" s="1"/>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A153" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A154" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A155" s="1"/>
+      <c r="A155" s="1" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A156" s="1" t="s">
-        <v>152</v>
-      </c>
+      <c r="A156" s="1"/>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A157" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A158" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A159" s="1"/>
+      <c r="A159" s="1" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A160" s="1" t="s">
-        <v>155</v>
-      </c>
+      <c r="A160" s="1"/>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A161" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A162" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A163" s="1"/>
+      <c r="A163" s="1" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A164" s="1" t="s">
-        <v>158</v>
-      </c>
+      <c r="A164" s="1"/>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A165" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A166" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A167" s="1"/>
+      <c r="A167" s="1" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A168" s="1" t="s">
-        <v>161</v>
-      </c>
+      <c r="A168" s="1"/>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A169" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A170" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A171" s="1"/>
+      <c r="A171" s="1" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A172" s="1" t="s">
-        <v>164</v>
-      </c>
+      <c r="A172" s="1"/>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A173" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A174" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A175" s="1"/>
+      <c r="A175" s="1" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A176" s="1" t="s">
-        <v>167</v>
-      </c>
+      <c r="A176" s="1"/>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A177" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A178" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A179" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A180" s="1" t="s">
-        <v>102</v>
-      </c>
+      <c r="A180" s="1"/>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A181" s="1"/>
+      <c r="A181" s="1" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A182" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A183" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A184" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A185" s="1" t="s">
-        <v>173</v>
+        <v>101</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A186" s="1" t="s">
-        <v>174</v>
-      </c>
+      <c r="A186" s="1"/>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A187" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A188" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A189" s="1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A190" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A191" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A192" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A193" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A194" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A195" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A196" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A197" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A198" s="1" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A199" s="1" t="s">
-        <v>99</v>
+        <v>181</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A200" s="1"/>
+      <c r="A200" s="1" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A201" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A202" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A203" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B203" t="s">
-        <v>9</v>
-      </c>
-      <c r="C203" t="s">
-        <v>104</v>
-      </c>
-      <c r="D203" t="s">
-        <v>11</v>
-      </c>
-      <c r="E203" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F203" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G203" t="s">
-        <v>39</v>
-      </c>
-      <c r="H203" t="s">
-        <v>103</v>
+        <v>183</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A204" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B204" t="s">
-        <v>9</v>
-      </c>
-      <c r="C204" t="s">
-        <v>104</v>
-      </c>
-      <c r="D204" t="s">
-        <v>11</v>
-      </c>
-      <c r="E204" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F204" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G204" t="s">
-        <v>39</v>
-      </c>
-      <c r="H204" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A205" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B205" t="s">
-        <v>9</v>
-      </c>
-      <c r="C205" t="s">
-        <v>104</v>
-      </c>
-      <c r="D205" t="s">
-        <v>11</v>
-      </c>
-      <c r="E205" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F205" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G205" t="s">
-        <v>39</v>
-      </c>
-      <c r="H205" t="s">
-        <v>103</v>
-      </c>
+      <c r="A205" s="1"/>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A206" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A207" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A208" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B206" t="s">
+      <c r="B208" t="s">
         <v>9</v>
       </c>
-      <c r="C206" t="s">
+      <c r="C208" t="s">
+        <v>103</v>
+      </c>
+      <c r="D208" t="s">
+        <v>11</v>
+      </c>
+      <c r="E208" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D206" t="s">
+      <c r="F208" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G208" t="s">
+        <v>38</v>
+      </c>
+      <c r="H208" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A209" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B209" t="s">
+        <v>9</v>
+      </c>
+      <c r="C209" t="s">
+        <v>103</v>
+      </c>
+      <c r="D209" t="s">
         <v>11</v>
       </c>
-      <c r="E206" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="F206" s="2" t="s">
+      <c r="E209" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="G206" t="s">
-        <v>39</v>
-      </c>
-      <c r="H206" t="s">
+      <c r="F209" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G209" t="s">
+        <v>38</v>
+      </c>
+      <c r="H209" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A210" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B210" t="s">
+        <v>9</v>
+      </c>
+      <c r="C210" t="s">
         <v>103</v>
+      </c>
+      <c r="D210" t="s">
+        <v>11</v>
+      </c>
+      <c r="E210" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F210" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G210" t="s">
+        <v>38</v>
+      </c>
+      <c r="H210" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A211" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B211" t="s">
+        <v>9</v>
+      </c>
+      <c r="C211" t="s">
+        <v>103</v>
+      </c>
+      <c r="D211" t="s">
+        <v>11</v>
+      </c>
+      <c r="E211" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F211" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G211" t="s">
+        <v>38</v>
+      </c>
+      <c r="H211" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>